<commit_message>
Prototyp + Paraphrasen überarbeitet
- Header neu erstellt
- Kalender: Titel hinzugefügt
</commit_message>
<xml_diff>
--- a/Auswertung_Fokusgruppen_01/Zusammenstellung der Kategorien.xlsx
+++ b/Auswertung_Fokusgruppen_01/Zusammenstellung der Kategorien.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cindy\Documents\GitHub\COMTRAC\Auswertung_Fokusgruppen_01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86718F3B-C5C6-48BA-95C0-E780C78E49FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614D1A47-940E-43DC-9134-2C05F4895B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{144474E4-DCCB-4C05-9FD5-E6CC91E1F337}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{144474E4-DCCB-4C05-9FD5-E6CC91E1F337}"/>
   </bookViews>
   <sheets>
     <sheet name="Auswertung Fokusgruppen" sheetId="1" r:id="rId1"/>
+    <sheet name="Anforderungen Symptomtagebuch" sheetId="2" r:id="rId2"/>
+    <sheet name="Anforderungen Medikation" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="67">
   <si>
     <t xml:space="preserve">Design </t>
   </si>
@@ -50,9 +52,6 @@
     <t>übersichtlich</t>
   </si>
   <si>
-    <t>Zusätzliche Funktionen</t>
-  </si>
-  <si>
     <t>Integration von Vitalparametern / Gesundheitszustand</t>
   </si>
   <si>
@@ -74,9 +73,6 @@
     <t>Gute Aufteilung</t>
   </si>
   <si>
-    <t xml:space="preserve">Bestehende Funktionen verbessern </t>
-  </si>
-  <si>
     <t>Rückmeldung bei Symptomeintrag</t>
   </si>
   <si>
@@ -108,12 +104,6 @@
   </si>
   <si>
     <t>Design</t>
-  </si>
-  <si>
-    <t>Zustätzliche Funktionen</t>
-  </si>
-  <si>
-    <t>Bestehende Funktionen verbessern</t>
   </si>
   <si>
     <t>Medikation</t>
@@ -278,16 +268,13 @@
     <t>Nutzen</t>
   </si>
   <si>
-    <t xml:space="preserve">Zusätzliche Funktionen: </t>
-  </si>
-  <si>
-    <t>Noch nicht im Prototyp vorhanden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bestehende Funktionen verbessern: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ablauf der Funktion verändert sich oder es wird was ergänzt oder gelöscht </t>
+    <t>Anpassung der Funktionen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anforderungen </t>
+  </si>
+  <si>
+    <t>Late Presenter</t>
   </si>
 </sst>
 </file>
@@ -324,7 +311,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,12 +330,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -362,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -379,9 +360,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF750585-B558-4ADB-8F8C-300D98D22696}">
-  <dimension ref="A2:H87"/>
+  <dimension ref="A2:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74:C74"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +705,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -720,15 +715,15 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -746,442 +741,583 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>9</v>
+      <c r="B9" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="E31" t="s">
-        <v>68</v>
-      </c>
-      <c r="G31" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" t="s">
-        <v>70</v>
-      </c>
-      <c r="H32" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="1" t="s">
-        <v>29</v>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
+      <c r="B38" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>47</v>
-      </c>
       <c r="B40" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>40</v>
-      </c>
+      <c r="A42" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>20</v>
+      <c r="C44" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>33</v>
-      </c>
+      <c r="A46" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>34</v>
-      </c>
       <c r="B47" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>2</v>
-      </c>
       <c r="B48" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>41</v>
+      <c r="B49" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>42</v>
+        <v>30</v>
+      </c>
+      <c r="B50" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-    </row>
-    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B52" s="1" t="s">
-        <v>35</v>
+      <c r="A51" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>48</v>
+      <c r="A54" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>2</v>
+      <c r="A57" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>44</v>
-      </c>
+      <c r="A58" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
+      <c r="A63" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>19</v>
+      <c r="A65" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
+      <c r="A67" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="B68" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>34</v>
-      </c>
-      <c r="B69" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>55</v>
+      <c r="C71" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>57</v>
-      </c>
+      <c r="A72" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C73" t="s">
-        <v>65</v>
+      <c r="A73" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>52</v>
+    <row r="75" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-    </row>
-    <row r="77" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>53</v>
+      <c r="A76" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B77" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>54</v>
+      <c r="B78" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B79" s="3" t="s">
-        <v>58</v>
+      <c r="B79" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B82" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B84" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C85" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B86" s="5"/>
-      <c r="C86" s="5"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>64</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="14">
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A74:C74"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A56:C56"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A74:C74"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A54:C54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EF07290-D813-4AE3-B209-F2CE025EB4A0}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="50.28515625" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10"/>
+      <c r="C10"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="C11"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B27D6BF-0EA5-441B-BBDF-89336BEB1FDE}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="50.28515625" style="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Bug behoben in "Main.cpp"
Verknüpfung zwischen QML und C++ muss über einen Pointer erstellt werden.
</commit_message>
<xml_diff>
--- a/Auswertung_Fokusgruppen_01/Zusammenstellung der Kategorien.xlsx
+++ b/Auswertung_Fokusgruppen_01/Zusammenstellung der Kategorien.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cindyhainz/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cindy\Documents\GitHub\COMTRAC\Auswertung_Fokusgruppen_01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B121AE20-0BC1-EB4D-9FC9-269D3B81777D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE690B8-9932-41C6-B518-B044F316648F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{144474E4-DCCB-4C05-9FD5-E6CC91E1F337}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{144474E4-DCCB-4C05-9FD5-E6CC91E1F337}"/>
   </bookViews>
   <sheets>
     <sheet name="Auswertung Fokusgruppen" sheetId="1" r:id="rId1"/>
@@ -382,7 +382,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,6 +401,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -414,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -435,15 +441,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="6"/>
     </xf>
@@ -459,6 +456,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -773,25 +780,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF750585-B558-4ADB-8F8C-300D98D22696}">
-  <dimension ref="A2:F119"/>
+  <dimension ref="A2:F116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="49.83203125" customWidth="1"/>
+    <col min="1" max="3" width="49.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -802,14 +809,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -817,7 +824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -825,88 +832,88 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>1</v>
       </c>
@@ -917,495 +924,491 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C32" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C33" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
       <c r="B40" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>30</v>
+      </c>
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" s="13"/>
+      <c r="C62" s="13"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-    </row>
-    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" t="s">
-        <v>35</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C44" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
+      <c r="B69" s="13"/>
+      <c r="C69" s="13"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B71" s="13"/>
+      <c r="C71" s="13"/>
+    </row>
+    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>50</v>
+      </c>
+      <c r="F73" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>55</v>
+      </c>
+      <c r="F75" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>57</v>
+      </c>
+      <c r="F77" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B79" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F79" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B84" s="14"/>
+      <c r="C84" s="14"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" s="13"/>
+      <c r="C88" s="13"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>30</v>
+      </c>
+      <c r="B90" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B91" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>30</v>
-      </c>
-      <c r="B50" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>2</v>
-      </c>
-      <c r="B51" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B92" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B95" s="13"/>
+      <c r="C95" s="13"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B97" s="13"/>
+      <c r="C97" s="13"/>
+    </row>
+    <row r="99" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1"/>
+      <c r="B101" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B102" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B103" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B104" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B105" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B106" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B107" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C108" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B111" s="14"/>
+      <c r="C111" s="14"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C112" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B65" s="9"/>
-      <c r="C65" s="9"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>30</v>
-      </c>
-      <c r="B67" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B69" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B70" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C71" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="9" t="s">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B72" s="9"/>
-      <c r="C72" s="9"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B74" s="9"/>
-      <c r="C74" s="9"/>
-    </row>
-    <row r="75" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>50</v>
-      </c>
-      <c r="F76" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B77" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B78" t="s">
-        <v>55</v>
-      </c>
-      <c r="F78" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B79" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B80" t="s">
-        <v>57</v>
-      </c>
-      <c r="F80" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B81" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B82" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F82" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C83" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B84" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B87" s="8"/>
-      <c r="C87" s="8"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B91" s="9"/>
-      <c r="C91" s="9"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>30</v>
-      </c>
-      <c r="B93" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B94" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B95" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B96" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C97" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B98" s="9"/>
-      <c r="C98" s="9"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B100" s="9"/>
-      <c r="C100" s="9"/>
-    </row>
-    <row r="102" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A102" s="14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A104" s="1"/>
-      <c r="B104" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B105" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B106" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B107" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B108" s="14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B109" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B110" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="C111" s="15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B113" s="13"/>
+      <c r="C113" s="13"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B114" s="8"/>
-      <c r="C114" s="8"/>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B116" s="9"/>
-      <c r="C116" s="9"/>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" s="11" t="s">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B119" s="11" t="s">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B116" s="8" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A116:C116"/>
-    <mergeCell ref="A87:C87"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="A98:C98"/>
-    <mergeCell ref="A100:C100"/>
-    <mergeCell ref="A114:C114"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A71:C71"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A53:C53"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="A113:C113"/>
+    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="A88:C88"/>
+    <mergeCell ref="A95:C95"/>
+    <mergeCell ref="A97:C97"/>
+    <mergeCell ref="A111:C111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1420,24 +1423,24 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="50.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="50.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="10"/>
-    </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C2" s="15"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -1448,47 +1451,47 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10"/>
       <c r="C10"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="C11"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14"/>
     </row>
   </sheetData>
@@ -1507,23 +1510,23 @@
       <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="50.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="50.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="10"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C2" s="15"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -1534,7 +1537,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>41</v>
       </c>
@@ -1542,7 +1545,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1550,7 +1553,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
@@ -1558,22 +1561,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1594,15 +1597,15 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="10"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -1629,15 +1632,15 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="10"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>

</xml_diff>